<commit_message>
1. Fixed issue 2. 2. Fixed bug that allowed for improper AllegroGraph uploading.
</commit_message>
<xml_diff>
--- a/sources/Ontologies.xlsx
+++ b/sources/Ontologies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liam9\Desktop\DSiP\Fair Trauma Reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liam9\Desktop\DSiP\Fair Trauma Reporting\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ADE2AB-EB57-44AC-9E45-ADEEE87611C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817303AF-2EA9-4704-927B-D3BC2FA55B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1958,7 +1958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC15B813-CE0B-46ED-83DD-9D8711974AE8}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>

</xml_diff>